<commit_message>
Cuadernillos 2 y 3 actividades adicionales
</commit_message>
<xml_diff>
--- a/Cuadernillos/results.xlsx
+++ b/Cuadernillos/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,10 +465,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -477,7 +477,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>1938</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="3">
@@ -485,10 +485,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
@@ -497,7 +497,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>3061</v>
+        <v>2975</v>
       </c>
     </row>
     <row r="4">
@@ -505,10 +505,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
@@ -517,6 +517,26 @@
         <v>1</v>
       </c>
       <c r="F4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>